<commit_message>
figures and experiment results
</commit_message>
<xml_diff>
--- a/excel/summary_diagrams.xlsx
+++ b/excel/summary_diagrams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="37920" windowHeight="19560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="k=1" sheetId="1" r:id="rId1"/>
@@ -616,11 +616,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2127077464"/>
-        <c:axId val="-2127069720"/>
+        <c:axId val="2144461304"/>
+        <c:axId val="2113363640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2127077464"/>
+        <c:axId val="2144461304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +663,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127069720"/>
+        <c:crossAx val="2113363640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -671,7 +671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127069720"/>
+        <c:axId val="2113363640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,7 +711,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127077464"/>
+        <c:crossAx val="2144461304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1449,11 +1449,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103188312"/>
-        <c:axId val="-2103182824"/>
+        <c:axId val="-2114976904"/>
+        <c:axId val="-2114969848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103188312"/>
+        <c:axId val="-2114976904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,11 +1466,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1482,7 +1486,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103182824"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2114969848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1490,7 +1504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103182824"/>
+        <c:axId val="-2114969848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,17 +1518,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF sal</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> 1 set in BF2</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1525,7 +1534,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103188312"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2114976904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1534,6 +1553,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -2253,11 +2282,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103150840"/>
-        <c:axId val="-2103145384"/>
+        <c:axId val="-2109567656"/>
+        <c:axId val="-2111161736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103150840"/>
+        <c:axId val="-2109567656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2270,11 +2299,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2286,7 +2319,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103145384"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2111161736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2294,7 +2337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103145384"/>
+        <c:axId val="-2111161736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2308,17 +2351,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in composed BF</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> 1 set in BF3</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2329,7 +2367,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103150840"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2109567656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2338,6 +2386,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -3057,11 +3115,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103113064"/>
-        <c:axId val="-2103107576"/>
+        <c:axId val="-2109509192"/>
+        <c:axId val="-2113265544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103113064"/>
+        <c:axId val="-2109509192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3074,11 +3132,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3090,7 +3152,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103107576"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2113265544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3098,7 +3170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103107576"/>
+        <c:axId val="-2113265544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3112,17 +3184,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of False Positive</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> False Positive</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3133,7 +3200,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103113064"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2109509192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3142,6 +3219,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -3861,11 +3948,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103078072"/>
-        <c:axId val="-2103072520"/>
+        <c:axId val="-2114066344"/>
+        <c:axId val="-2101230552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103078072"/>
+        <c:axId val="-2114066344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3878,11 +3965,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3894,7 +3985,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103072520"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2101230552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3902,7 +4003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103072520"/>
+        <c:axId val="-2101230552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3916,17 +4017,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF emp</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> 1 set in BF1</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3937,7 +4033,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103078072"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2114066344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3946,6 +4052,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -4665,11 +4781,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103059320"/>
-        <c:axId val="-2103053848"/>
+        <c:axId val="-2105712600"/>
+        <c:axId val="-2116338664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103059320"/>
+        <c:axId val="-2105712600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4682,11 +4798,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4698,7 +4818,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103053848"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2116338664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4706,7 +4836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103053848"/>
+        <c:axId val="-2116338664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4720,17 +4850,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF sal</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> 1 set in BF2</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4741,7 +4866,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103059320"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2105712600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4750,6 +4885,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -5469,11 +5614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103996072"/>
-        <c:axId val="-2103992488"/>
+        <c:axId val="-2109620680"/>
+        <c:axId val="-2117673288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103996072"/>
+        <c:axId val="-2109620680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5486,11 +5631,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5502,7 +5651,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103992488"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2117673288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5510,7 +5669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103992488"/>
+        <c:axId val="-2117673288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5524,15 +5683,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> 1 set in BF3</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in composed BF</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5544,7 +5699,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103996072"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2109620680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5553,6 +5718,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -6272,11 +6447,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103977208"/>
-        <c:axId val="-2103971720"/>
+        <c:axId val="-2110931080"/>
+        <c:axId val="-2109636952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103977208"/>
+        <c:axId val="-2110931080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6289,11 +6464,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6305,7 +6484,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103971720"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2109636952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6313,7 +6502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103971720"/>
+        <c:axId val="-2109636952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6327,17 +6516,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of False Positive</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> False Positive</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6348,7 +6532,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103977208"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2110931080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6357,6 +6551,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -6836,11 +7040,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122388264"/>
-        <c:axId val="-2122382776"/>
+        <c:axId val="-2107177784"/>
+        <c:axId val="-2108720616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122388264"/>
+        <c:axId val="-2107177784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6853,11 +7057,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom FIlter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6869,7 +7077,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122382776"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2108720616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6877,7 +7095,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122382776"/>
+        <c:axId val="-2108720616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6891,17 +7109,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF sal</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> of 1 set</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6912,7 +7125,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122388264"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2107177784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6921,6 +7144,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -7400,11 +7633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122351000"/>
-        <c:axId val="-2122345432"/>
+        <c:axId val="2145481192"/>
+        <c:axId val="2145486792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122351000"/>
+        <c:axId val="2145481192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7447,7 +7680,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122345432"/>
+        <c:crossAx val="2145486792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7455,7 +7688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122345432"/>
+        <c:axId val="2145486792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7495,7 +7728,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122351000"/>
+        <c:crossAx val="2145481192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7554,7 +7787,7 @@
             <c:v>Collected Data</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="19050"/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -7772,7 +8005,7 @@
             <c:v>Expected Values</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="19050"/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -7993,11 +8226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123285816"/>
-        <c:axId val="-2123291320"/>
+        <c:axId val="-2121649960"/>
+        <c:axId val="-2116531848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123285816"/>
+        <c:axId val="-2121649960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8010,11 +8243,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8026,7 +8263,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123291320"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2116531848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8034,7 +8281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123291320"/>
+        <c:axId val="-2116531848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8048,10 +8295,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
+                  <a:rPr lang="de-DE" sz="2000"/>
                   <a:t>Number of False Positive</a:t>
                 </a:r>
               </a:p>
@@ -8064,7 +8311,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123285816"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2121649960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8073,6 +8330,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -8792,11 +9059,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123341528"/>
-        <c:axId val="-2123347032"/>
+        <c:axId val="2144155656"/>
+        <c:axId val="2144161592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123341528"/>
+        <c:axId val="2144155656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8809,22 +9076,37 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123347032"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2144161592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8832,7 +9114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123347032"/>
+        <c:axId val="2144161592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8846,29 +9128,51 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of 1 set BF1</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF emp</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123341528"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2144155656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -9588,11 +9892,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103322632"/>
-        <c:axId val="-2103317144"/>
+        <c:axId val="-2119613976"/>
+        <c:axId val="-2119611656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103322632"/>
+        <c:axId val="-2119613976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9605,22 +9909,37 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103317144"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2119611656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9628,7 +9947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103317144"/>
+        <c:axId val="-2119611656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9642,29 +9961,51 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of 1 set BF2</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF sal</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103322632"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2119613976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -10384,11 +10725,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103285464"/>
-        <c:axId val="-2103279976"/>
+        <c:axId val="-2102171096"/>
+        <c:axId val="-2102125192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103285464"/>
+        <c:axId val="-2102171096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10401,22 +10742,37 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103279976"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2102125192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10424,7 +10780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103279976"/>
+        <c:axId val="-2102125192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10438,29 +10794,51 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of 1 set BF3</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in composed BF</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103285464"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2102171096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -11180,11 +11558,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2079547112"/>
-        <c:axId val="2079542232"/>
+        <c:axId val="2140502088"/>
+        <c:axId val="2140712280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2079547112"/>
+        <c:axId val="2140502088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11197,22 +11575,37 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079542232"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140712280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11220,7 +11613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079542232"/>
+        <c:axId val="2140712280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11234,34 +11627,51 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of False Positive</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> False Positive</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079547112"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140502088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -11981,11 +12391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103234536"/>
-        <c:axId val="-2103229048"/>
+        <c:axId val="-2105082136"/>
+        <c:axId val="2145348056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103234536"/>
+        <c:axId val="-2105082136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11998,11 +12408,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Bloom Filter Size in Bit</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Bloom Filter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+                  <a:t> Size in Bit</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -12014,7 +12428,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103229048"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2145348056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12022,7 +12446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103229048"/>
+        <c:axId val="2145348056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12036,17 +12460,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Number of</a:t>
+                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:t>Number of 1 set in BF emp</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> 1 set in BF1</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -12057,7 +12476,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103234536"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2105082136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12066,6 +12495,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -12113,16 +12552,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12173,15 +12612,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -12208,16 +12647,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12238,16 +12677,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12268,16 +12707,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12298,16 +12737,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12333,16 +12772,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12363,16 +12802,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12393,16 +12832,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12423,16 +12862,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12458,16 +12897,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12488,16 +12927,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12518,16 +12957,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12548,16 +12987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12903,8 +13342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT19" workbookViewId="0">
-      <selection activeCell="AV35" sqref="AV35"/>
+    <sheetView topLeftCell="AO17" workbookViewId="0">
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14461,8 +14900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ14"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="B14" activeCellId="1" sqref="B6:AZ6 B14:AZ14"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AY24" sqref="AY24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16074,7 +16513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ14"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
+    <sheetView topLeftCell="AB1" workbookViewId="0">
       <selection activeCell="B14" activeCellId="1" sqref="B6:AZ6 B14:AZ14"/>
     </sheetView>
   </sheetViews>
@@ -17687,7 +18126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ14"/>
   <sheetViews>
-    <sheetView topLeftCell="AK10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z5" workbookViewId="0">
       <selection activeCell="B14" activeCellId="1" sqref="B6:AZ6 B14:AZ14"/>
     </sheetView>
   </sheetViews>

</xml_diff>